<commit_message>
material expense. 17 test cases accomplished.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/material_expense_record_test_cases.xlsx
+++ b/soberano/test_cases/material_expense_record_test_cases.xlsx
@@ -287,11 +287,11 @@
   </sheetPr>
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G49" activeCellId="0" sqref="G49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="18:18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.11"/>
@@ -894,7 +894,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
material expense recording completed. disabling in progress. adding rounding to quantity and amount (#.########)
</commit_message>
<xml_diff>
--- a/soberano/test_cases/material_expense_record_test_cases.xlsx
+++ b/soberano/test_cases/material_expense_record_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="52">
   <si>
     <t xml:space="preserve">TC Number</t>
   </si>
@@ -154,22 +154,28 @@
     <t xml:space="preserve">l</t>
   </si>
   <si>
+    <t xml:space="preserve">It fails due to wrong values since user 18 is a salesclerk. Hence, user 18 can not retrieve  providers, materials, so can't populate the corresponding combos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unauthorized user18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorized user1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It fails due to not enough rights.</t>
+  </si>
+  <si>
     <t xml:space="preserve">It fails due to negative values.</t>
   </si>
   <si>
-    <t xml:space="preserve">Unauthorized user18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authorized user1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It fails due to not enough rights.</t>
+    <t xml:space="preserve">check recorded expenses</t>
   </si>
 </sst>
 </file>
@@ -251,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,6 +271,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,13 +295,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="18:18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.11"/>
@@ -820,7 +830,7 @@
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -1005,7 +1015,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>45</v>
@@ -1259,7 +1269,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>45</v>
@@ -1402,7 +1412,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>37</v>
@@ -1437,7 +1447,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>48</v>
@@ -1475,7 +1485,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>41</v>
@@ -1513,7 +1523,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>45</v>
@@ -1621,7 +1631,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>37</v>
@@ -1766,8 +1776,8 @@
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>49</v>
+      <c r="B41" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>45</v>
@@ -1805,7 +1815,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>37</v>
@@ -1843,7 +1853,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>41</v>
@@ -1915,8 +1925,8 @@
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="0" t="s">
-        <v>49</v>
+      <c r="B45" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>45</v>
@@ -1954,7 +1964,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>37</v>
@@ -1988,8 +1998,8 @@
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>49</v>
+      <c r="B47" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>45</v>
@@ -2055,6 +2065,14 @@
       </c>
       <c r="L48" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>